<commit_message>
Fixt Edit Profile test
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -130,9 +130,6 @@
     <t>AvailableTime</t>
   </si>
   <si>
-    <t>Full time</t>
-  </si>
-  <si>
     <t>Mera</t>
   </si>
   <si>
@@ -142,13 +139,16 @@
     <t>Hours</t>
   </si>
   <si>
-    <t>More than 30hours a week</t>
-  </si>
-  <si>
     <t>EarnTarget</t>
   </si>
   <si>
-    <t>Between $500 and $1000 per month</t>
+    <t>Full Time</t>
+  </si>
+  <si>
+    <t>As needed</t>
+  </si>
+  <si>
+    <t>More than $1000 per month</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -763,24 +763,24 @@
         <v>36</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
-        <v>39</v>
-      </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
         <v>43</v>

</xml_diff>

<commit_message>
Edit the Skill share
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn" sheetId="1" r:id="rId1"/>
     <sheet name="SignUp" sheetId="2" r:id="rId2"/>
     <sheet name="SkillShareAdd" sheetId="3" r:id="rId3"/>
     <sheet name="Profile" sheetId="4" r:id="rId4"/>
+    <sheet name="EditShareSkill" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="56">
   <si>
     <t>Url</t>
   </si>
@@ -161,6 +162,30 @@
   </si>
   <si>
     <t>LocationType</t>
+  </si>
+  <si>
+    <t>OldTitle</t>
+  </si>
+  <si>
+    <t>OldDescription</t>
+  </si>
+  <si>
+    <t>SkillExchange</t>
+  </si>
+  <si>
+    <t>test2</t>
+  </si>
+  <si>
+    <t>New Skill Share</t>
+  </si>
+  <si>
+    <t>I love automation testing</t>
+  </si>
+  <si>
+    <t>Graphics &amp; Design</t>
+  </si>
+  <si>
+    <t>Flyers &amp; Brochures</t>
   </si>
 </sst>
 </file>
@@ -634,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -650,6 +675,8 @@
     <col min="11" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -786,7 +813,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -842,4 +869,161 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:S3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="5">
+        <v>43534</v>
+      </c>
+      <c r="K2" s="5">
+        <v>43554</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="3">
+        <v>10</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19">
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>